<commit_message>
working on other income
</commit_message>
<xml_diff>
--- a/database design.xlsx
+++ b/database design.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7305"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -235,9 +235,6 @@
     <t>other_income</t>
   </si>
   <si>
-    <t>id,company_id,purpose,payment_type_id,description,amount,user_id,time</t>
-  </si>
-  <si>
     <t>company,payment_type,user</t>
   </si>
   <si>
@@ -284,6 +281,9 @@
   </si>
   <si>
     <t>company,shelf,supplier,generic,strength,medicine_type,user</t>
+  </si>
+  <si>
+    <t>id,company_id,purpose,date,payment_type_id,description,amount,user_id,time</t>
   </si>
 </sst>
 </file>
@@ -323,7 +323,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -333,6 +333,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -364,7 +370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -385,6 +391,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -691,24 +701,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="50.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.7265625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="50.54296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.26953125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.5">
       <c r="C2" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
@@ -722,7 +732,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="4" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>1</v>
       </c>
@@ -730,13 +740,13 @@
         <v>4</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>2</v>
       </c>
@@ -744,25 +754,25 @@
         <v>70</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="4" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="6"/>
       <c r="B8" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>86</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>87</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A9" s="7">
         <v>3</v>
       </c>
@@ -770,41 +780,41 @@
         <v>71</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="9" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="A10" s="8">
         <v>4</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D10" s="7" t="s">
+    </row>
+    <row r="11" spans="1:4" s="9" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="A11" s="8">
+        <v>5</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
-        <v>5</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="4" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:4" s="4" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <v>6</v>
       </c>
@@ -818,7 +828,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" s="4" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
         <v>7</v>
       </c>
@@ -832,7 +842,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A14" s="6">
         <v>8</v>
       </c>
@@ -846,7 +856,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A15" s="7">
         <v>9</v>
       </c>
@@ -860,7 +870,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" s="4" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="6">
         <v>10</v>
       </c>
@@ -874,7 +884,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
         <v>11</v>
       </c>
@@ -888,7 +898,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" s="4" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="6">
         <v>12</v>
       </c>
@@ -902,7 +912,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A19" s="7">
         <v>13</v>
       </c>
@@ -916,7 +926,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A20" s="7">
         <v>14</v>
       </c>
@@ -930,7 +940,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A21" s="7">
         <v>15</v>
       </c>
@@ -938,41 +948,41 @@
         <v>28</v>
       </c>
       <c r="C21" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A22" s="7">
+    </row>
+    <row r="22" spans="1:4" s="9" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="8">
         <v>16</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="7">
+    <row r="23" spans="1:4" s="9" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="A23" s="8">
         <v>17</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A24" s="7">
         <v>18</v>
       </c>
@@ -986,7 +996,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A25" s="7">
         <v>19</v>
       </c>
@@ -1000,7 +1010,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A26" s="7">
         <v>20</v>
       </c>
@@ -1014,7 +1024,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A27" s="7">
         <v>21</v>
       </c>
@@ -1028,7 +1038,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A28" s="7">
         <v>22</v>
       </c>
@@ -1042,7 +1052,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:4" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" s="4" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="6">
         <v>23</v>
       </c>
@@ -1056,7 +1066,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="62" x14ac:dyDescent="0.35">
       <c r="A30" s="7">
         <v>24</v>
       </c>
@@ -1070,7 +1080,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A31" s="7">
         <v>25</v>
       </c>
@@ -1084,7 +1094,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A32" s="7">
         <v>26</v>
       </c>
@@ -1098,7 +1108,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="62" x14ac:dyDescent="0.35">
       <c r="A33" s="7">
         <v>27</v>
       </c>
@@ -1106,13 +1116,13 @@
         <v>57</v>
       </c>
       <c r="C33" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D33" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D33" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A34" s="7">
         <v>28</v>
       </c>
@@ -1126,7 +1136,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A35" s="7">
         <v>29</v>
       </c>
@@ -1140,7 +1150,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A36" s="7">
         <v>30</v>
       </c>
@@ -1154,15 +1164,15 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A37" s="7">
         <v>31</v>
       </c>
       <c r="B37" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" s="7" t="s">
         <v>77</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>78</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
working on tuktak 2
</commit_message>
<xml_diff>
--- a/database design.xlsx
+++ b/database design.xlsx
@@ -701,8 +701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -772,17 +772,17 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="7">
+    <row r="9" spans="1:4" s="4" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="6">
         <v>3</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>83</v>
       </c>
     </row>

</xml_diff>

<commit_message>
working on medicine purchase
</commit_message>
<xml_diff>
--- a/database design.xlsx
+++ b/database design.xlsx
@@ -124,18 +124,9 @@
     <t>purchase</t>
   </si>
   <si>
-    <t>id,company_id,purchase_code,supplier_id,invoice_no,purchase_date,details,vat,total_amount,total_discount,net_payable,status,user_id,time</t>
-  </si>
-  <si>
     <t>company,supplier,user</t>
   </si>
   <si>
-    <t>purchase_history</t>
-  </si>
-  <si>
-    <t>id,company_id,purchase_id,supplier_id,medicine_id,qty,supplier_price,vat,total_amount,discount,net_amount,espire_date,user_id,status,time</t>
-  </si>
-  <si>
     <t>company,purchase,supplier,medicine,user</t>
   </si>
   <si>
@@ -284,6 +275,15 @@
   </si>
   <si>
     <t>id,company_id,medicine_code,name,shelf_id,supplier_id,batch_no,generic_id,strength_id,medicine_type_id,box_size,box_price,mrp,trade_price,vat,p_discount,details,side_effect,in_stock,short_stock,favourite,isDiscount,sale_quantity,user_id,status,time</t>
+  </si>
+  <si>
+    <t>id,company_id,purchase_code,supplier_id,invoice_no,purchase_date,details,vat,total_amount,total_discount,net_payable,user_id,time</t>
+  </si>
+  <si>
+    <t>id,company_id,purchase_id,supplier_id,medicine_id,qty,supplier_price,vat,total_amount,discount,net_amount,expire_date,user_id,time</t>
+  </si>
+  <si>
+    <t>purchase_details</t>
   </si>
 </sst>
 </file>
@@ -323,7 +323,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -339,6 +339,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -370,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -395,6 +401,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -701,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -715,7 +724,7 @@
   <sheetData>
     <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.5">
       <c r="C2" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
@@ -729,7 +738,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
@@ -740,7 +749,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>7</v>
@@ -751,22 +760,22 @@
         <v>2</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="4" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="6"/>
       <c r="B8" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>31</v>
@@ -777,13 +786,13 @@
         <v>3</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="9" customFormat="1" ht="31" x14ac:dyDescent="0.35">
@@ -791,13 +800,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="9" customFormat="1" ht="31" x14ac:dyDescent="0.35">
@@ -805,13 +814,13 @@
         <v>5</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="4" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
@@ -912,46 +921,46 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A19" s="7">
+    <row r="19" spans="1:4" s="9" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="A19" s="8">
         <v>13</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A20" s="7">
+    <row r="20" spans="1:4" s="9" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="A20" s="8">
         <v>14</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="77.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="7">
+    <row r="21" spans="1:4" s="9" customFormat="1" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="8">
         <v>15</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>87</v>
+      <c r="C21" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="9" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
@@ -983,72 +992,72 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="7">
+      <c r="A24" s="6">
         <v>18</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="7" t="s">
+    </row>
+    <row r="25" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="8">
+        <v>19</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="7">
-        <v>19</v>
-      </c>
-      <c r="B25" s="7" t="s">
+    <row r="26" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="A26" s="8">
+        <v>20</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C26" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D26" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A26" s="7">
-        <v>20</v>
-      </c>
-      <c r="B26" s="7" t="s">
+    <row r="27" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="6">
+        <v>21</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C27" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D27" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="A28" s="6">
+        <v>22</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="7">
-        <v>21</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A28" s="7">
-        <v>22</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D28" s="7" t="s">
+      <c r="C28" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="6" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1057,55 +1066,55 @@
         <v>23</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="62" x14ac:dyDescent="0.35">
-      <c r="A30" s="7">
+      <c r="A30" s="10">
         <v>24</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="31" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A31" s="7">
+      <c r="A31" s="6">
         <v>25</v>
       </c>
-      <c r="B31" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C31" s="7" t="s">
+      <c r="B31" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="6">
+        <v>26</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D32" s="6" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="7">
-        <v>26</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="62" x14ac:dyDescent="0.35">
@@ -1113,13 +1122,13 @@
         <v>27</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="31" x14ac:dyDescent="0.35">
@@ -1127,13 +1136,13 @@
         <v>28</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
@@ -1141,13 +1150,13 @@
         <v>29</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
@@ -1155,13 +1164,13 @@
         <v>30</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
@@ -1169,10 +1178,10 @@
         <v>31</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>1</v>

</xml_diff>